<commit_message>
add pay u code in purchase
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelResultsFolder/s2sResults.xlsx
+++ b/src/test/resources/ExcelResultsFolder/s2sResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\integrationApiUiTesting\src\test\resources\ExcelResultsFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6BB5E-427B-4B7F-95E6-742561DFA143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05842790-BA21-4AF9-B279-B17675B44E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,16 @@
     <sheet name="StreetAddress_Result" sheetId="5" r:id="rId5"/>
     <sheet name="Zipcode_Result" sheetId="6" r:id="rId6"/>
     <sheet name="Statecode_Result" sheetId="7" r:id="rId7"/>
+    <sheet name="Currency_Result" sheetId="8" r:id="rId8"/>
+    <sheet name="Productname_Result" sheetId="9" r:id="rId9"/>
+    <sheet name="BrandID_Result" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="580">
   <si>
     <t>ProductName</t>
   </si>
@@ -1142,6 +1145,630 @@
   </si>
   <si>
     <t>2025-12-15 16:26:48</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>693ffb8c2a49368b7dd96b18</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:49:21</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>693ffcda2a49368b7dd96dcf</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:50:19</t>
+  </si>
+  <si>
+    <t>inr</t>
+  </si>
+  <si>
+    <t>693ffd272a49368b7dd9708a</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:51:34</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly JPY</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:52:07</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly XYZ</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:52:21</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly ABC</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:52:36</t>
+  </si>
+  <si>
+    <t>usd</t>
+  </si>
+  <si>
+    <t>693ffd982a49368b7dd9736f</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:58:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> US D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS → currency rejected correctly  US D </t>
+  </si>
+  <si>
+    <t>2025-12-15 17:58:22</t>
+  </si>
+  <si>
+    <t>US1</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly US1</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:58:39</t>
+  </si>
+  <si>
+    <t>EU@</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly EU@</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:58:56</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly 123</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:59:13</t>
+  </si>
+  <si>
+    <t>@#$</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly @#$</t>
+  </si>
+  <si>
+    <t>2025-12-15 17:59:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS → currency rejected correctly </t>
+  </si>
+  <si>
+    <t>2025-12-15 17:59:43</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly null</t>
+  </si>
+  <si>
+    <t>2025-12-15 18:00:01</t>
+  </si>
+  <si>
+    <t>USDIND</t>
+  </si>
+  <si>
+    <t>PASS → currency rejected correctly USDIND</t>
+  </si>
+  <si>
+    <t>2025-12-15 18:00:17</t>
+  </si>
+  <si>
+    <t>6940057f2a49368b7dd97ccd</t>
+  </si>
+  <si>
+    <t>2025-12-15 18:31:51</t>
+  </si>
+  <si>
+    <t>694006d12a49368b7dd98171</t>
+  </si>
+  <si>
+    <t>2025-12-15 18:32:53</t>
+  </si>
+  <si>
+    <t>694018982a49368b7dd9872e</t>
+  </si>
+  <si>
+    <t>2025-12-15 19:50:19</t>
+  </si>
+  <si>
+    <t>694019572a49368b7dd989c8</t>
+  </si>
+  <si>
+    <t>2025-12-15 19:51:58</t>
+  </si>
+  <si>
+    <t>69412f63457a500e47fffc25</t>
+  </si>
+  <si>
+    <t>2025-12-16 15:39:44</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>694131e9457a500e470005ed</t>
+  </si>
+  <si>
+    <t>2025-12-16 15:53:36</t>
+  </si>
+  <si>
+    <t>69413260457a500e47000894</t>
+  </si>
+  <si>
+    <t>2025-12-16 15:55:40</t>
+  </si>
+  <si>
+    <t>694137a89023226b5ff8c4ef</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:13:33</t>
+  </si>
+  <si>
+    <t>6941381d9023226b5ff8c791</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:15:27</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>694138629023226b5ff8ca32</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:16:38</t>
+  </si>
+  <si>
+    <t>694138ab9023226b5ff8ccf2</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:17:45</t>
+  </si>
+  <si>
+    <t>694138fd9023226b5ff8d004</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:19:13</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>694139479023226b5ff8d2b0</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:20:25</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>6941398e9023226b5ff8d557</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:21:32</t>
+  </si>
+  <si>
+    <t>694139d19023226b5ff8d809</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:22:40</t>
+  </si>
+  <si>
+    <t>ZZ</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly ZZ</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:23:09</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly XYZ</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:23:21</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly IND</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:23:33</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly India</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:23:44</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:23:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN </t>
+  </si>
+  <si>
+    <t>69413a509023226b5ff8dd69</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:24:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IN</t>
+  </si>
+  <si>
+    <t>69413a929023226b5ff8e377</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:25:53</t>
+  </si>
+  <si>
+    <t>IN 1</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly IN 1</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:26:22</t>
+  </si>
+  <si>
+    <t>@N</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly @N</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:26:34</t>
+  </si>
+  <si>
+    <t>PASS → country rejected correctly 123</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:26:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS → country rejected correctly </t>
+  </si>
+  <si>
+    <t>2025-12-16 16:26:58</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:27:10</t>
+  </si>
+  <si>
+    <t>69413cc69023226b5ff8e99f</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:35:23</t>
+  </si>
+  <si>
+    <t>69413d129023226b5ff8ec61</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:36:35</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:37:04</t>
+  </si>
+  <si>
+    <t>69413e259023226b5ff8ef75</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:40:42</t>
+  </si>
+  <si>
+    <t>69413e489023226b5ff8f20e</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:41:49</t>
+  </si>
+  <si>
+    <t>69413f469023226b5ff8f845</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:45:38</t>
+  </si>
+  <si>
+    <t>69413f709023226b5ff8fad7</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:46:44</t>
+  </si>
+  <si>
+    <t>69413fc39023226b5ff8fd89</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:48:06</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:48:40</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:48:53</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:49:07</t>
+  </si>
+  <si>
+    <t>694140389023226b5ff90055</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:49:33</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:49:52</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:50:05</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:50:17</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:50:30</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:50:44</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:50:57</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:51:09</t>
+  </si>
+  <si>
+    <t>2025-12-16 16:51:22</t>
+  </si>
+  <si>
+    <t>858D754D-106A-4C1D-B36A-820D82C84B8B</t>
+  </si>
+  <si>
+    <t>69414ef42d8e3e88fc9d46a2</t>
+  </si>
+  <si>
+    <t>2025-12-16 17:54:20</t>
+  </si>
+  <si>
+    <t>858d754d-106a-41-b36a-82082c84b8b</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly 858d754d-106a-41-b36a-82082c84b8b</t>
+  </si>
+  <si>
+    <t>2025-12-16 17:58:22</t>
+  </si>
+  <si>
+    <t>858d754d-106a-4c1d-b36a-820d82c84b8b</t>
+  </si>
+  <si>
+    <t>694150872d8e3e88fc9d4ec6</t>
+  </si>
+  <si>
+    <t>2025-12-16 17:59:43</t>
+  </si>
+  <si>
+    <t>694150d72d8e3e88fc9d5444</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:01:03</t>
+  </si>
+  <si>
+    <t>694151272d8e3e88fc9d56f3</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:02:21</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:02:53</t>
+  </si>
+  <si>
+    <t>858d754d-106a4c1db36a820d82c84b8b</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly 858d754d-106a4c1db36a820d82c84b8b</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:03:06</t>
+  </si>
+  <si>
+    <t>858d754d-106a-4c1d-b36a-820d82c84b8b123</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly 858d754d-106a-4c1d-b36a-820d82c84b8b123</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:03:19</t>
+  </si>
+  <si>
+    <t>858d754d-106a-4c1d-b36a-820d82c84b8bz</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly 858d754d-106a-4c1d-b36a-820d82c84b8bz</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:03:32</t>
+  </si>
+  <si>
+    <t>@@@d858d754d-106a-4c1d-b36a-820d82c84b8b</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly @@@d858d754d-106a-4c1d-b36a-820d82c84b8b</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:03:46</t>
+  </si>
+  <si>
+    <t>huagsuyush</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly huagsuyush</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:04:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS → brandid rejected correctly </t>
+  </si>
+  <si>
+    <t>2025-12-16 18:04:12</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly null</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:04:25</t>
+  </si>
+  <si>
+    <t>aaaaaaaa-bbbb-cccc-dddd-eeeeeeeeeeee</t>
+  </si>
+  <si>
+    <t>PASS → brandid rejected correctly aaaaaaaa-bbbb-cccc-dddd-eeeeeeeeeeee</t>
+  </si>
+  <si>
+    <t>2025-12-16 18:04:37</t>
+  </si>
+  <si>
+    <t>6942a88340e6a841067be71f</t>
+  </si>
+  <si>
+    <t>2025-12-17 18:27:07</t>
+  </si>
+  <si>
+    <t>6942a8c240e6a841067bec7d</t>
+  </si>
+  <si>
+    <t>2025-12-17 18:28:05</t>
+  </si>
+  <si>
+    <t>6942a8fd40e6a841067bef64</t>
+  </si>
+  <si>
+    <t>2025-12-17 18:29:05</t>
+  </si>
+  <si>
+    <t>6943a0219a3b87c1f14e8905</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:03:21</t>
+  </si>
+  <si>
+    <t>6943a0589a3b87c1f14e8b9a</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:04:16</t>
+  </si>
+  <si>
+    <t>6943a0ef9a3b87c1f14e913b</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:06:46</t>
+  </si>
+  <si>
+    <t>6943a5c99a3b87c1f14e9bd4</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:27:29</t>
+  </si>
+  <si>
+    <t>6943a6ea9a3b87c1f14ea1e9</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:32:17</t>
+  </si>
+  <si>
+    <t>6943aaff9a3b87c1f14eae1b</t>
+  </si>
+  <si>
+    <t>2025-12-18 12:49:43</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>69450c44089896a1804fd209</t>
+  </si>
+  <si>
+    <t>2025-12-19 13:57:00</t>
+  </si>
+  <si>
+    <t>69452bb516b84676a86cf20c</t>
+  </si>
+  <si>
+    <t>2025-12-19 16:11:05</t>
+  </si>
+  <si>
+    <t>69452c1a16b84676a86cf757</t>
+  </si>
+  <si>
+    <t>2025-12-19 16:12:44</t>
+  </si>
+  <si>
+    <t>6948d469311f13a333ea395c</t>
+  </si>
+  <si>
+    <t>2025-12-22 10:47:50</t>
+  </si>
+  <si>
+    <t>6948d5d7311f13a333ea3c0a</t>
+  </si>
+  <si>
+    <t>2025-12-22 10:53:46</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>6948d759311f13a333ea4289</t>
+  </si>
+  <si>
+    <t>2025-12-22 11:00:12</t>
+  </si>
+  <si>
+    <t>6948d89a311f13a333ea4786</t>
+  </si>
+  <si>
+    <t>2025-12-22 11:05:39</t>
+  </si>
+  <si>
+    <t>6948d9aa311f13a333ea4a0b</t>
+  </si>
+  <si>
+    <t>2025-12-22 11:10:11</t>
+  </si>
+  <si>
+    <t>6948d9f7311f13a333ea4c70</t>
+  </si>
+  <si>
+    <t>2025-12-22 11:11:28</t>
+  </si>
+  <si>
+    <t>6948dcb3311f13a333ea5406</t>
+  </si>
+  <si>
+    <t>2025-12-22 11:23:07</t>
   </si>
 </sst>
 </file>
@@ -1637,6 +2264,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.1796875"/>
+    <col min="2" max="2" customWidth="true" width="20.54296875"/>
+    <col min="3" max="3" customWidth="true" width="78.26953125"/>
+    <col min="4" max="4" customWidth="true" width="29.08984375"/>
+    <col min="5" max="5" customWidth="true" width="30.36328125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>505</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>507</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>508</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>510</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>511</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>513</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>515</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>507</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>508</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>518</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>519</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>521</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>522</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>524</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>525</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>527</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>528</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>530</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>531</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>533</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>535</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>537</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>538</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>539</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E24"/>
@@ -1980,7 +2851,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
         <v>179</v>
       </c>
@@ -1997,15 +2868,13 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="0"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s" s="0">
         <v>23</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>283</v>
       </c>
-      <c r="D24" s="0"/>
       <c r="E24" t="s" s="0">
         <v>369</v>
       </c>
@@ -2017,9 +2886,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2277,7 +3146,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
         <v>53</v>
       </c>
@@ -2294,7 +3163,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
         <v>56</v>
       </c>
@@ -2304,22 +3173,258 @@
       <c r="C18" t="s" s="0">
         <v>293</v>
       </c>
-      <c r="D18" s="0"/>
       <c r="E18" t="s" s="0">
         <v>365</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="0"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s" s="0">
         <v>23</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>295</v>
       </c>
-      <c r="D19" s="0"/>
       <c r="E19" t="s" s="0">
         <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>437</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s" s="0">
+        <v>439</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>440</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>443</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>344</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>445</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>447</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>448</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>450</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s" s="0">
+        <v>452</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>453</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>455</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>459</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>460</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>462</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>463</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s" s="0">
+        <v>465</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>466</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s" s="0">
+        <v>468</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>469</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>473</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -2329,7 +3434,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -2649,7 +3754,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
         <v>205</v>
       </c>
@@ -2666,7 +3771,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
         <v>75</v>
       </c>
@@ -2681,6 +3786,108 @@
       </c>
       <c r="E21" t="s" s="0">
         <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>430</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>433</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>435</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>540</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>542</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>544</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -2690,9 +3897,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -3629,7 +4836,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
         <v>100</v>
       </c>
@@ -3644,6 +4851,17 @@
       </c>
       <c r="E59" t="s" s="0">
         <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="E60" t="s" s="0">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -3653,11 +4871,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.0"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="24.7265625"/>
+    <col min="4" max="4" customWidth="true" width="26.6328125"/>
+    <col min="5" max="5" customWidth="true" width="29.08984375"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
@@ -3742,6 +4967,40 @@
       </c>
       <c r="E5" t="s" s="0">
         <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>476</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>478</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -3753,7 +5012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -4298,4 +5557,956 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.90625"/>
+    <col min="2" max="2" customWidth="true" width="17.0"/>
+    <col min="3" max="3" customWidth="true" width="38.26953125"/>
+    <col min="4" max="4" customWidth="true" width="27.453125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>376</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>378</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>382</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>384</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>389</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>390</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>392</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>393</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>395</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>396</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>398</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>399</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>403</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>404</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>410</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>411</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>413</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>415</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>417</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>419</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>421</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>481</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>483</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>485</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>487</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s" s="0">
+        <v>378</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>489</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>382</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>384</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>389</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>494</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s" s="0">
+        <v>392</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>393</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s" s="0">
+        <v>395</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>396</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s" s="0">
+        <v>398</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>399</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s" s="0">
+        <v>403</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>404</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s" s="0">
+        <v>410</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>411</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>546</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>548</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>550</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>552</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>554</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>556</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>558</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>559</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>561</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>563</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>565</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>567</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>570</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>572</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>574</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>576</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>578</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>579</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.7265625"/>
+    <col min="2" max="2" customWidth="true" width="13.90625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>423</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>424</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>423</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>426</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>423</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>428</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
zaakpay Integration & Easybuzz is done
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelResultsFolder/s2sResults.xlsx
+++ b/src/test/resources/ExcelResultsFolder/s2sResults.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\integrationApiUiTesting\src\test\resources\ExcelResultsFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD0770D-4286-4804-8F10-7403D6D39685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDC41BE-FC04-4C48-B798-71E864359EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StateCode" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="249">
   <si>
     <t>Test Data</t>
   </si>
@@ -782,13 +782,18 @@
   </si>
   <si>
     <t>2025-12-31 11:06:02</t>
+  </si>
+  <si>
+    <t>69566345d115b7038739053e</t>
+  </si>
+  <si>
+    <t>2026-01-01 17:37:12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1167,11 +1172,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="17.26953125"/>
-    <col min="3" max="3" customWidth="true" width="23.81640625"/>
-    <col min="4" max="4" customWidth="true" width="15.453125"/>
-    <col min="5" max="5" customWidth="true" width="12.81640625"/>
-    <col min="6" max="6" customWidth="true" width="15.81640625"/>
+    <col min="1" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1235,709 +1240,709 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.7265625"/>
-    <col min="3" max="3" customWidth="true" width="18.08984375"/>
-    <col min="4" max="4" customWidth="true" width="44.54296875"/>
-    <col min="5" max="5" customWidth="true" width="38.453125"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" customWidth="1"/>
+    <col min="5" max="5" width="38.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s" s="0">
+      <c r="F11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s" s="0">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s" s="0">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s" s="0">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s" s="0">
+      <c r="F13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s" s="0">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="F14" t="s" s="0">
+      <c r="F14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s" s="0">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" t="s" s="0">
+      <c r="F15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s" s="0">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s" s="0">
+      <c r="F16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s" s="0">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s" s="0">
+      <c r="F17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s" s="0">
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="F18" t="s" s="0">
+      <c r="F18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s" s="0">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="F19" t="s" s="0">
+      <c r="F19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s" s="0">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s" s="0">
+      <c r="F20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s" s="0">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" t="s" s="0">
+      <c r="F21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s" s="0">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" t="s" s="0">
+      <c r="F22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s" s="0">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s" s="0">
+      <c r="F23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s" s="0">
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>49</v>
       </c>
-      <c r="F24" t="s" s="0">
+      <c r="F24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s" s="0">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
         <v>51</v>
       </c>
-      <c r="F25" t="s" s="0">
+      <c r="F25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s" s="0">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s" s="0">
+      <c r="F26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s" s="0">
+      <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s" s="0">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
         <v>55</v>
       </c>
-      <c r="F27" t="s" s="0">
+      <c r="F27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s" s="0">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s" s="0">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
         <v>57</v>
       </c>
-      <c r="F28" t="s" s="0">
+      <c r="F28" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B29" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D29" t="s" s="0">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
         <v>59</v>
       </c>
-      <c r="F29" t="s" s="0">
+      <c r="F29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s" s="0">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B30" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D30" t="s" s="0">
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
         <v>20</v>
       </c>
-      <c r="E30" t="s" s="0">
+      <c r="E30" t="s">
         <v>61</v>
       </c>
-      <c r="F30" t="s" s="0">
+      <c r="F30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s" s="0">
+      <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s" s="0">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
         <v>51</v>
       </c>
-      <c r="F31" t="s" s="0">
+      <c r="F31" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s" s="0">
+      <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s" s="0">
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s" s="0">
+      <c r="F32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s" s="0">
+      <c r="A33" t="s">
         <v>27</v>
       </c>
-      <c r="B33" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s" s="0">
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>55</v>
       </c>
-      <c r="F33" t="s" s="0">
+      <c r="F33" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s" s="0">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s" s="0">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
         <v>57</v>
       </c>
-      <c r="F34" t="s" s="0">
+      <c r="F34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B35" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s" s="0">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
         <v>59</v>
       </c>
-      <c r="F35" t="s" s="0">
+      <c r="F35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s" s="0">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="B36" t="s" s="0">
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D36" t="s" s="0">
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
         <v>20</v>
       </c>
-      <c r="E36" t="s" s="0">
+      <c r="E36" t="s">
         <v>87</v>
       </c>
-      <c r="F36" t="s" s="0">
+      <c r="F36" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s" s="0">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B37" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s" s="0">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
         <v>89</v>
       </c>
-      <c r="F37" t="s" s="0">
+      <c r="F37" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s" s="0">
+      <c r="A38" t="s">
         <v>24</v>
       </c>
-      <c r="B38" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s" s="0">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
         <v>89</v>
       </c>
-      <c r="F38" t="s" s="0">
+      <c r="F38" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s" s="0">
+      <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="B39" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s" s="0">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
         <v>89</v>
       </c>
-      <c r="F39" t="s" s="0">
+      <c r="F39" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s" s="0">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
-      <c r="B40" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s" s="0">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
         <v>89</v>
       </c>
-      <c r="F40" t="s" s="0">
+      <c r="F40" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B41" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s" s="0">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
         <v>89</v>
       </c>
-      <c r="F41" t="s" s="0">
+      <c r="F41" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1948,228 +1953,253 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="A5:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.90625"/>
-    <col min="2" max="2" customWidth="true" width="17.36328125"/>
-    <col min="3" max="3" customWidth="true" width="17.08984375"/>
-    <col min="4" max="4" customWidth="true" width="42.36328125"/>
-    <col min="5" max="5" customWidth="true" width="31.1796875"/>
+    <col min="1" max="1" width="20.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="4" max="4" width="42.36328125" customWidth="1"/>
+    <col min="5" max="5" width="31.1796875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>79</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>81</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>72</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>85</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>240</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>241</v>
       </c>
-      <c r="G8" t="s" s="0">
+      <c r="G8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>243</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>241</v>
       </c>
-      <c r="G9" t="s" s="0">
+      <c r="G9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>245</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>241</v>
       </c>
-      <c r="G10" t="s" s="0">
+      <c r="G10" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2187,198 +2217,198 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="22.36328125"/>
-    <col min="4" max="4" customWidth="true" width="42.08984375"/>
-    <col min="5" max="5" customWidth="true" width="38.90625"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="42.08984375" customWidth="1"/>
+    <col min="5" max="5" width="38.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>96</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>99</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>102</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>104</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>105</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>107</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>108</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>112</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>113</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>115</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>117</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>119</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>120</v>
       </c>
-      <c r="F11" t="s" s="0">
+      <c r="F11" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2397,408 +2427,408 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.453125"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" customWidth="true" width="14.81640625"/>
-    <col min="4" max="4" customWidth="true" width="50.0"/>
-    <col min="5" max="5" customWidth="true" width="36.08984375"/>
-    <col min="6" max="6" customWidth="true" width="30.453125"/>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+    <col min="5" max="5" width="36.08984375" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>123</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>125</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>126</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>128</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>129</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>132</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>134</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>135</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>137</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>138</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>140</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>141</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>143</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>144</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>146</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>147</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>149</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>150</v>
       </c>
-      <c r="F11" t="s" s="0">
+      <c r="F11" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>152</v>
       </c>
-      <c r="B12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s" s="0">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
         <v>153</v>
       </c>
-      <c r="F12" t="s" s="0">
+      <c r="F12" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>155</v>
       </c>
-      <c r="B13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s" s="0">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>156</v>
       </c>
-      <c r="F13" t="s" s="0">
+      <c r="F13" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>158</v>
       </c>
-      <c r="B14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s" s="0">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
         <v>159</v>
       </c>
-      <c r="F14" t="s" s="0">
+      <c r="F14" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="B15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s" s="0">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
         <v>162</v>
       </c>
-      <c r="F15" t="s" s="0">
+      <c r="F15" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>164</v>
       </c>
-      <c r="B16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s" s="0">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>165</v>
       </c>
-      <c r="F16" t="s" s="0">
+      <c r="F16" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>167</v>
       </c>
-      <c r="B17" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s" s="0">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
         <v>168</v>
       </c>
-      <c r="F17" t="s" s="0">
+      <c r="F17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>170</v>
       </c>
-      <c r="B18" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s" s="0">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
         <v>171</v>
       </c>
-      <c r="F18" t="s" s="0">
+      <c r="F18" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>173</v>
       </c>
-      <c r="B19" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s" s="0">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>174</v>
       </c>
-      <c r="F19" t="s" s="0">
+      <c r="F19" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>176</v>
       </c>
-      <c r="B20" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s" s="0">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
         <v>177</v>
       </c>
-      <c r="F20" t="s" s="0">
+      <c r="F20" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>179</v>
       </c>
-      <c r="B21" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s" s="0">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
         <v>180</v>
       </c>
-      <c r="F21" t="s" s="0">
+      <c r="F21" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s" s="0">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>182</v>
       </c>
-      <c r="F22" t="s" s="0">
+      <c r="F22" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s" s="0">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>184</v>
       </c>
-      <c r="F23" t="s" s="0">
+      <c r="F23" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2811,84 +2841,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="41.1796875"/>
-    <col min="5" max="5" customWidth="true" width="36.54296875"/>
+    <col min="4" max="4" width="41.1796875" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>186</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>187</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>189</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>191</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2908,93 +2938,93 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>193</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>194</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>196</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>197</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>199</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>201</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3013,279 +3043,279 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="40.6328125"/>
-    <col min="5" max="5" customWidth="true" width="33.81640625"/>
+    <col min="4" max="4" width="40.6328125" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>203</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>205</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>207</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>208</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>210</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>211</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>203</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>205</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>207</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>208</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>196</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>216</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>218</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>72</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>219</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>205</v>
       </c>
-      <c r="F11" t="s" s="0">
+      <c r="F11" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>207</v>
       </c>
-      <c r="B12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s" s="0">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
         <v>208</v>
       </c>
-      <c r="F12" t="s" s="0">
+      <c r="F12" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s" s="0">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>203</v>
       </c>
-      <c r="F13" t="s" s="0">
+      <c r="F13" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s" s="0">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
         <v>205</v>
       </c>
-      <c r="F14" t="s" s="0">
+      <c r="F14" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>207</v>
       </c>
-      <c r="B15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s" s="0">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
         <v>208</v>
       </c>
-      <c r="F15" t="s" s="0">
+      <c r="F15" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s" s="0">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>203</v>
       </c>
-      <c r="F16" t="s" s="0">
+      <c r="F16" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3304,156 +3334,156 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="25.90625"/>
-    <col min="4" max="4" customWidth="true" width="42.453125"/>
-    <col min="5" max="5" customWidth="true" width="33.0"/>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>222</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>224</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>225</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>221</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>230</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>224</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>232</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>205</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>207</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>208</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>203</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>239</v>
       </c>
     </row>

</xml_diff>